<commit_message>
adding all sathish files
</commit_message>
<xml_diff>
--- a/Testdata/TC_Chart_86.xlsx
+++ b/Testdata/TC_Chart_86.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksathish\git\cucumber\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speriyasamy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="My Series" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -33,7 +33,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Dh8AAB+LCAAAAAAAAAOlWVtv48YV/iuEniuRlGXLEsYMZMl2hEi2YWnrdV+KETmyp6ZIlUPa1tuiaJItWrRoUzRoUyDtSzcPaRGkWyTtbvJr1va+7V/omQuvkmvTXRhrzjnfOTNz5txmjN67mrnaBQkY9b2tilkzKhrxbN+h3ulWJQqnVXOj8p6Fdq5s4h7iAM9ICGANpDzWvmJ0q3IWhvO2rl9eXtYu12p+cKrXDcPUnw4HI/uMzHCVeizEnk0qiZRzv1TFQl1nNiQhdnCIpeRWpT/q17qE2j2gDbGHT0lQ244Y9QhjO15IQ0oYlwwIDkm3N/yh3JhVr23UTKQv0VPkdkRdR+JySElXOJiWjOmMWHWjblSNVtWoj4319nqrbTZq5kb9R7FgAkQDzMIRCS6oLQijEM/mQtxowX/r6y2zgfSVINCVGsBCB65zRC4oI06XuC4rZRFdHWDHDmHX5YxpID0jqxQ9fgl7AZ6fjWnokrLiu35AbDDUo+beJ5cHgbLfeD4A7viMBuGihxeldT1hJDiYc2uUE7VQz/fCjkuC8MkcDpU4cObAsMIgIki/g5kK9Siz4Zt6EXGsKXZZVijHRMd+cM7m2Cb7ELA613HpuT52wLNCykJqp5MuMdBh4M9BI0y+7bvOLmhV4BWMRHPfAxPzabd9/zxd3SomEj4gvAHOdIbDGL5ER6Mz//LAcxejaMLsgE6I09uO0St5iEeeku5GLPRnsIqUhCQtQ1nAP4i0Ihn1iE1n2D10wYjMghjNE1AnCv0pDbu+G808Fq+pQEXHsKMxuUp2mIzRARyux43ue30vxkszr2TlBY78y2TOZYYwQobcYXZ83MuMIrgHtPj4ljniRPgud6kLhSB7Fhlq3itGZ4SEK11CchDPebu8tFgd10V6OkTgluDasAzLgOpQFT9jw2iLH5g2YaMdz7kbFzPRfjQ7mED4XogNWSbwCiQEW3C3XeydA/WYhmf7nXjpKzhIbvhO/DIPQaDOXbwQ5MQoWRrqe7YbOUTGf9+bCo/ka5NneCcbLZEGENIWwt5ivJhDvmW0HcLHVgUqcJuFAdT4imX7kRcGC54okK6g98mwaOKJCbD7YJlpQH4aQWux2I08u+s7D5/NkdZ54tHw4Sv0o0Bmv4eLCOvxRBixHuEpReT4B8vbZfbEglLwmUdmvkfth1sbjMxX7zxiIyyOqgdLEBlfD8a7UMZlleOx/mCxAPpCqGulpukw5ttUOKsKDycjr98RMj0yxZELPVkIFfU0SbVFMuqw8yImS0JPAjdOeBbveBm0vLYzq9nQK/C2rmb7M07QodM8HiE9i+cNj012vNMB9k4jaCmSvFKkJ+mWl8NxgD3Gt5N0EIXMuxqE4jwlOxtLJq+DSDiCTF4+cJFewKExmc39ALtDMAzdVW6n2iPoPIY4PFMjKGUusWMj66loIpVfWbzw+2CiJslt8IBXabJAFCC+F9lcp5iUhvguhxCWbhe7dBLIrBpX7lU8OLC0F4zzL99cyb4wPgO4YEGx/YAseNedDhRduKwZM6QD80RqjY6ajQ3DWIMuRYyR2PE+CbUBRCZ4os6/t/0g8C9hBDVPWERVnfvAWRjajbO4mKgDq8lT8gBoHk4pFIllYMJJBawTggN3kQHKjQx8G3BvX35z8+X31x8/u372+ub5H66ffZ4M5X4kDI3xxCViKePtumk26hvgQAkNcavposV1IjsUtP5IdLbJGKmbmBh0d/rdvcG2SBQJMRaXtULnl7yFH6XDkVy/mEiclR4fsYRY4zjxqHGOm6k9Fr90XZA8Osu/S1Aa4/bVi9tXf79TWlksbaLMVqtZNev39lh1w2wt4ZIea5BL7uqqvFldy4ILGHQkM3tip75jra0319cazc1mkqSdxGVXgYospWmMT/WCnCR1Zd+TuEB2HDOFz/fhPoI9J0HIQMgMpB2vP/rq+uvPcihlYEVZUgRLFF0Kn1KPB0J7ehvTEqEMOwOVU7yPT+H+MsVan3Ewy6LVIpKgyrmX50XY/YEmA1+rwB2novlTjWD7TFtAOGaCMed2q6hyokeqLK5yL/CjuTiLk4xASl2BTFLKSokVCUfwhEGXMk/KWgFX5/3vl6sE1EZ6ac8K3vWBNvMSDxU0lONIUoav4veP37/59mPpWNcf/vLmz5/mlKipkrs+OD2EVnaYxADkP1VVChR0PBL2PDd+nKkiisivS4c+9UJm1dfETUmNEIiaXJv4jfozKGxCsTAZ0AsU9D5mO1ehinJrH+l5AqxzjqGm+umFMiHIjJ4pBH/9QuuPah3DbL57/SdIRQacxM2XL25efv325d9unn/z5rtPbv/56t3r5zujjsb5717/ApDXn313/dGHt7///M1/Xtw8ewV1gxN/9sXbT35+/btfQSWRFUZVi2JFEdsQX/HkbS3W39b2eodtbYQveNOnQQBqmXKaUcj3KTqYYtaQy7v56re3r35z869f3/zl29t/fMqNUEBn5eN00tb21VVM69jiMsdykomQbBW6a+ba5lqCUFXRn1N7OZUVyCksTWUpSXJl5T2ESeoNxZVT8A5oglnGsHuuP4FFxwzx3FCA5KT+t0CKFfPtDQ62O4MUIhdxEDgk4P4pP1CfxT1l7HcZCnCh17Mjl78KLcGWWSj+yqQ1XT2vTDsO94XVrxM5BOpGQSC7JE89y4+iOfS/8SPc3XzxMJlpefdle5ptgtNxv5fnwzjDhRKZZ3OC4ItUpVgybfUZf8mRHew+N006BF7uMRPMoV7eZQ92QeEYdJ6EdqDdDFZmopQTw4bQPEN60VOLJxidTykbbSc9q5gQZ7/kQ1721A79HnFJWPpZOpYe+hePloWzLyvaZweuo4xZ7raRmCVVkH2b545SdjGdIIDmij/mlX5MH1DvvF9u95bZdOot06iv1zfJxIZPZ7NurDcbDnGM1hpvL4VSfvnkKmbQgfOrW8lJkJ4XT6/ZR3DxLqlNGlgI8qsoWEoEJBfi19B4jHZpwMKnPEWpL0k5SSgnssF+ytcnP8T4xGpsSgIA9Oxkem7VcX4J5Z9xfHdAZ7TkddWIk1BeCbjBfC77zrIH2u0N98lViPSMBsjWk59AkZLvO2W0yaiCJJ/Ix7pG0aS0Oj0WPgQ+d6zHSe840LA9Xlr8UYS6/8cCREv2WBV9j9HTs7DsuTaajlFvTJvVBjbtamOzZVRbZt2pYnNqNM36Zmtzw+EP2ko5VAdKLktOwmsKZXDnKC+nF/6qbf0XrSQsCg4fAAA=</t>
+          <t>TCEAAB+LCAAAAAAAAAPNWt1vG8cR/1cIPpe845EUSWF9AUVKChFSEky6tvtSLO+W0lXHO/b2ThLfjLZOXPS7bhu0KZD2pfZDGhipi6Sxk7/GpPzmf6GzX/dBUjDPyEMMA76d+c3s7OzszOzS6L2rqVu4IAF1fO9WsVLWiwXiWb7teKe3ilE4KVV2iu+ZaP/KIu4JDvCUhAAugJRHd6+oc6t4FoazXU27vLwsX1bLfnCqGbpe0e4N+kPrjExxyfFoiD2LFGMp++1SRRN17OmAhNjGIRaSt4q9Ya/cIY7VBdoAe/iUBOW9iDoeoXTfC53QIZRJBgSHpNMd/FAszDTKO+UK0tboCXIvclxb4DJIQZc4mJaMnCkxDd2olPRKqdIc6fVdvbprNMrVncaPlGAMRH1MwyEJLhyLE4Yhns64uF6pNPW6XjUaSNsIAl2JA0x07Nq3yYVDid0hrktzeUSTG9i2Qlh1PmfqSEvJSkXvbsJhgGdnIyd0SV7xAz8gFjjqneY+IpfHgfTfaNYH7ujMCcJ5F89z67pDSXA8Y97IJ2qiru+FbZcE4Z0ZbCqxYc+BYYZBRJB2AzMR6jrUgm/Hi4htTrBL00IZJrrrB+d0hi1yBAdWYzouPdfHNkRW6NDQsZJJ1xjoJPBnoBEm3/Nd+wC0SvAGRqy554GL2bR7vn+eWLeJiXgM8GiAPZ3iUMHX6Gh45l8ee+58GI2pFThjYnf3FHojD7GTJ6U7EQ39KViRkJCgpSiDgWbb2hz+wHlbZaIusZwpdk9ccCU1DdCVIaB2FPoTJ+z4bjT1qLJshYruwrpG5CpeZzxGx7DFHnO97/U8hRfO3sjKCtz2L+M51xncFSlym1pq09cZq+Au0NQmrnP4vrBVHjgulIP0jqSo2dgYnhESbgwMwUEs8x2wAmO2XRdpyRBBcEKAgxmmDjWixP+OdH2X/4VpYzba9+ybcYqJjqLp8RgO8QVfkFkB3goJwRLcPRd750C964RnR21l+gYOEgu+Eb/OQ3BcZy6ec3LslDQN9TzLjWwiskDPm/CIZLaJPbyRjdZIfTjYJsLefDSfQdalzm4IH7eKUId3aRhApS+alh95YTBn6QJpEvo2GRqNPT4BdreWmQTkpxE0GPODyLM6vr39bLbwzh3PCbe30I8CkQO3F+HeY+kwol3CEgvP9FvLW3nWRINc8KlHpr7nWNt7G5zMrLffYSFUnaqtJYg4X1vjXSjmotaxs761WADdIVS3XNO0KfUthwerPB52Sl674ch0yQRHLnRmIdTV0zjVrpJRm56vYtIkdCdwVcIzWd9LofG17GnZgo6BNXdly58yggb95t0h0tJ41vZYZN877WPvNILGIs4rq/Q43bKiOAqwR9ly4j5iJfNuBiGVp0R/Y4rkdRzxQBDJywcu0lZwaESmMz/A7gAc4xzIsJNNEvQfAxyeyRGUMpdYyslaIhpLZS1Thr8NxmuSWAY78DJNrhA5iK1FtNgJJqEhtsoBHEu3g11nHIisqir3Jh5sWNIRqvzLFpezO1R7ANcsKLYfkDnrvZOBpPOQrSiGCGCWSM3h7UZtR9erNWhk2BjxFR+RsNCHkwmRqLHvPT8I/EsYQc3jHpFV523gNAwdqCzOJ2qDNVlKFgDNw6kDRWIdGHMSAfM+wYE7TwHFQvq+BbjXz79cfvbt4qMHiwcvl4/+snjwaTwU6xEwNMJjl3BTRntGpVIzdiCAYhpiXtN4o2tHVshpvSHvb+MxkvcxPujs9zqH/T2eKGKiEhe1QmNXvbkfJcOhsJ9PxPdKU1ssIOZIJR45znBTtcdkV68LkkWn+TcJCmdcv3hy/eLfN0pLjyVNVKXVqpcqxlt7LEOvtNZwcY/VzyR3duPVObiZAq9g0G2R2WM/9WyzWm/Uq7VGsxEnaTsO2U2gVZbUNMKn2oqcIHVE3xOHQHqsmDzme3ArwZ4dI8RBSA2EHxcfPlt88UkGJR0sKWuKwETepbApNTXg2pM7WSEWSrFTUDHF+/gU7i8TXOhRBqZptDQiPlSZ8PK8CLs/KIiDXyjCHadY8CcFgq2zwhyOY+owZsJuE1VM9I4qV608DPxoxvfifkogoW5Axillo8SGhMN53KFrmSdhbYDL/f7f800CciHdpGeF6PqgMPXiCOU0lOEIUoovz+9fv3311UcisBYPf7X8+8cZJXKq+MYPQQ9HKz2MzwDkP1lVVijo7pD781z/caqKSCK7Lp34jhfCBbjOb0pyhEC0wrTxf1FvCoWNK+YuA/oKBb2P6f5VKE+5eYS0LAHsnGGoqX5yoYwJIqOnCsE/nxZ6w3JbN6pvXv4NUpEOO7H87Mny+Revn/9r+ejLV988vv7PizcvH+0P2wXGf/Pyl4BcfPLN4sOH13/69NXXT5YPXkDdYMSfPX39+BeLP/4aKomoMLJarFYUvgz+pSbfLSj9u4XD7sluYYgvWNNXgANYSJXTlEK2Tt7BrGYNYd7y2R+uX/xu+d/fLv/x1fXnHzMnrKDT8iqd7BaO5FWs0Lb4ZY5mJGMh0Sp0qpVqsxojZFX0Z461nspWyAksSWUJSXBF5T2BSYya5IopWAc0xjTl2MXDp9e///nyz8+Wv/l88fVj/tywAslImYeuP4ZVKlpWIMHy+Q77x3vtfgIRRhwHNglYfIoP1KOqp1Rxl6IAF3o9K3LZq9AabJ2F1FcqrWnyeWXStlksbH6dyCBQJwoC0SV58nF+GM2g/1VPcTfz+fNkquU9Eu1puglOxr1ulg/jFBdKZJbNCJzPU5VkibTVo+wlR3SwR8w1yRB4mSdNcId8fxc92IUD26CxJLQP7WawMRMlHAUbQPMM6UVLPB5jNDalaLTtZK8UQWW/+ENc9uQK/S5xSZj7cVpJD/yLd5aFvc8r2qPHri2dme+2EbslUZB+oWeBkteYdhBAc8Ue83I/qfcd77yXb/Vm3W40muO6NR5PDMPA42bLqlcnrYbVqE2qZALtJVfKLp9MxRQ6cHZ1yzcJ3Fiy4sk1+zZcvHNqEw7mguwqCp6S7/MHTkDDeywnyS9BuR9T7ouO+h4zSHzw8X2zLvtoAGhp7VrGTJVQQvHrje/2namT836qq6yTVQL7PpuJRjPvDna6gyNyFSItpQHS8/gnUJXEg04ubWdwRYGkHosrVcNonF+bC2OlTCpQ+k5AhMVWPoXq4YeGAMg+/TT1BmlY1UZpTKxxqVatjUvNsdUo6fV6Q99pthrjuq5dOOSSaq2KbkxaTQIXKdso1YhFSi2r1SwRw8IQ+7Zt4ApAKXTfVKtUx7Y1qdilxoTslGpGfVIa60arVG1OGg2rNraq2FBrVItSi9y3obX8Lhc5hcuyC8lfGKcR0J/LQGVQbCD/nchxv9utwDNHu1Ae3Mo+zZYHLTY0bZiylrfC3wNryzPWi26wif3gQJ3TszDvId4meNnPFVI51H4I5LyTbBP2SBOa2QzMH3nn2C4YlW6VbpP/E2H+H0I+abNMIQAA</t>
         </r>
       </text>
     </comment>
@@ -44,7 +44,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
-    <t>Select this link and click Refresh/Edit Download to update data and add or remove series</t>
+    <t>Select this link and click Refresh to update data for this chart</t>
   </si>
   <si>
     <t>Net Lending/Net Borrowing</t>
@@ -147,12 +147,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +185,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -220,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,9 +224,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,16 +530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -638,7 +625,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="4">
-        <v>35765</v>
+        <v>35034</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -654,7 +641,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="5">
-        <v>44074</v>
+        <v>44173</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -674,7 +661,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>-39247.814839207393</v>
+        <v>-34223.287304702411</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +669,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="2">
-        <v>18950904369.08902</v>
+        <v>18542203593.64854</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +677,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="2">
-        <v>137662.2837566231</v>
+        <v>136169.7602026549</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +685,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="2">
-        <v>-0.32891976020032437</v>
+        <v>-0.31712883123902091</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +693,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>-3.3959757578383432E-2</v>
+        <v>8.3705198118324553E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +701,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="2">
-        <v>-3.5075146048412011</v>
+        <v>-3.9788626671156941</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +709,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="2">
-        <v>-351961.95977474999</v>
+        <v>-351152.00370264001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +717,7 @@
         <v>30</v>
       </c>
       <c r="B24" s="2">
-        <v>186780.03305616</v>
+        <v>197931.06711860999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +725,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="2">
-        <v>-43633.938548949998</v>
+        <v>-43209.800590810002</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,191 +733,207 @@
         <v>32</v>
       </c>
       <c r="B26" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <v>35765</v>
+        <v>35034</v>
       </c>
       <c r="B27" s="8">
-        <v>-12825.260670739999</v>
+        <v>571</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>36130</v>
-      </c>
-      <c r="B28" s="8">
-        <v>-43633.938548949998</v>
+        <v>35400</v>
+      </c>
+      <c r="B28" s="9">
+        <v>-12288</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>36495</v>
-      </c>
-      <c r="B29" s="8">
-        <v>-46424.812615629999</v>
+        <v>35765</v>
+      </c>
+      <c r="B29" s="9">
+        <v>-12811.4818574</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>36861</v>
-      </c>
-      <c r="B30" s="8">
-        <v>-72631.308023610007</v>
+        <v>36130</v>
+      </c>
+      <c r="B30" s="9">
+        <v>-43611.084733889998</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>37226</v>
-      </c>
-      <c r="B31" s="8">
-        <v>-34562.241340979999</v>
+        <v>36495</v>
+      </c>
+      <c r="B31" s="9">
+        <v>-46397.102240009997</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>37591</v>
+        <v>36861</v>
       </c>
       <c r="B32" s="9">
-        <v>9300.6227574099994</v>
+        <v>-72556.106552269994</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>37956</v>
-      </c>
-      <c r="B33" s="8">
-        <v>-43243.192800700002</v>
+        <v>37226</v>
+      </c>
+      <c r="B33" s="9">
+        <v>-34436.689569349997</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>38322</v>
+        <v>37591</v>
       </c>
       <c r="B34" s="8">
-        <v>-95081.256552520004</v>
+        <v>10015.47751561</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>38687</v>
-      </c>
-      <c r="B35" s="8">
-        <v>-167415.35055189001</v>
+        <v>37956</v>
+      </c>
+      <c r="B35" s="9">
+        <v>-43209.800590810002</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>39052</v>
-      </c>
-      <c r="B36" s="8">
-        <v>-279160.67288937001</v>
+        <v>38322</v>
+      </c>
+      <c r="B36" s="9">
+        <v>-97873.512601830007</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>39417</v>
-      </c>
-      <c r="B37" s="8">
-        <v>-191620.49408251001</v>
+        <v>38687</v>
+      </c>
+      <c r="B37" s="9">
+        <v>-167106.31250624001</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <v>39783</v>
-      </c>
-      <c r="B38" s="8">
-        <v>-351961.95977474999</v>
+        <v>39052</v>
+      </c>
+      <c r="B38" s="9">
+        <v>-278847.36862437002</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>40148</v>
-      </c>
-      <c r="B39" s="8">
-        <v>-154798.55685354999</v>
+        <v>39417</v>
+      </c>
+      <c r="B39" s="9">
+        <v>-191229.77625056001</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>40513</v>
-      </c>
-      <c r="B40" s="8">
-        <v>-108328.63309957999</v>
+        <v>39783</v>
+      </c>
+      <c r="B40" s="9">
+        <v>-351152.00370264001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
-        <v>40878</v>
-      </c>
-      <c r="B41" s="8">
-        <v>-91117.938830769999</v>
+        <v>40148</v>
+      </c>
+      <c r="B41" s="9">
+        <v>-167442.02989010001</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>41244</v>
-      </c>
-      <c r="B42" s="8">
-        <v>-71580.070182790005</v>
+        <v>40513</v>
+      </c>
+      <c r="B42" s="9">
+        <v>-108042.82745373</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>41609</v>
+        <v>40878</v>
       </c>
       <c r="B43" s="9">
-        <v>111716.74491633</v>
+        <v>-90926.49041174</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <v>41974</v>
+        <v>41244</v>
       </c>
       <c r="B44" s="9">
-        <v>79834.374744419998</v>
+        <v>-71389.391172060001</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>42339</v>
-      </c>
-      <c r="B45" s="9">
-        <v>116659.31024331</v>
+        <v>41609</v>
+      </c>
+      <c r="B45" s="8">
+        <v>113092.02433273999</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>42705</v>
-      </c>
-      <c r="B46" s="9">
-        <v>186780.03305616</v>
+        <v>41974</v>
+      </c>
+      <c r="B46" s="8">
+        <v>87376.435711800004</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>43070</v>
-      </c>
-      <c r="B47" s="10">
-        <v>97618.447737659997</v>
+        <v>42339</v>
+      </c>
+      <c r="B47" s="8">
+        <v>125987.38721643</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>43435</v>
-      </c>
-      <c r="B48" s="10">
-        <v>86329.962615910001</v>
+        <v>42705</v>
+      </c>
+      <c r="B48" s="8">
+        <v>197931.06711860999</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
+        <v>43070</v>
+      </c>
+      <c r="B49" s="8">
+        <v>107728.96249957</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>43435</v>
+      </c>
+      <c r="B50" s="8">
+        <v>101555.55762879</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>43800</v>
       </c>
-      <c r="B49" s="10">
-        <v>181770.44944537</v>
+      <c r="B51" s="8">
+        <v>189479.88351588999</v>
       </c>
     </row>
   </sheetData>
@@ -943,14 +946,14 @@
 <MetadataExcelFile xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
   <MetadataLink>
     <MetadataLink>
-      <SheetId>My Series</SheetId>
-      <LinkPosRow>1</LinkPosRow>
+      <SheetId>Chart</SheetId>
+      <LinkPosRow>22</LinkPosRow>
       <LinkPosCol>1</LinkPosCol>
       <MetaDataSeries>
         <MetadataSeries>
-          <InitRow>1</InitRow>
+          <InitRow>22</InitRow>
           <InitCol>2</InitCol>
-          <EndRow>49</EndRow>
+          <EndRow>72</EndRow>
           <EndCol>2</EndCol>
           <Name>Net Lending/Net Borrowing</Name>
           <DisplayName>Net Lending/Net Borrowing</DisplayName>
@@ -965,7 +968,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1617F-2980-40CC-8683-B6C1063890D6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE411C81-2BAB-4121-BEB7-46DCF41C80C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
   </ds:schemaRefs>

</xml_diff>